<commit_message>
Update spreadsheet for feet
</commit_message>
<xml_diff>
--- a/data/human_measurements.xlsx
+++ b/data/human_measurements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="1300" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Weight" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="166">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>Roll (Degree)</t>
+  </si>
+  <si>
+    <t>Cylinder Radius</t>
   </si>
 </sst>
 </file>
@@ -4145,8 +4148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4203,7 +4206,8 @@
         <v>-8.5500000000000007E-2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>K4</f>
+        <v>0.02</v>
       </c>
       <c r="E2">
         <f>B2+$K$2</f>
@@ -4215,7 +4219,7 @@
       </c>
       <c r="G2">
         <f>D2+$M$2</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K2" s="15">
         <v>0.76987700000000003</v>
@@ -4238,7 +4242,8 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f>-B2</f>
+        <v>-4.0999999999999995E-2</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E20" si="0">B3+$K$2</f>
@@ -4250,7 +4255,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G20" si="2">D3+$M$2</f>
-        <v>0</v>
+        <v>-4.0999999999999995E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -4266,7 +4271,8 @@
         <v>8.5500000000000007E-2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f>K4</f>
+        <v>0.02</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -4278,7 +4284,13 @@
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.02</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4">
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4292,7 +4304,8 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f>-B4</f>
+        <v>-4.0999999999999995E-2</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -4304,7 +4317,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-4.0999999999999995E-2</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -5058,7 +5071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use joint centers where possible for k-chain
</commit_message>
<xml_diff>
--- a/data/human_measurements.xlsx
+++ b/data/human_measurements.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="9840" yWindow="340" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Weight" sheetId="1" r:id="rId1"/>
@@ -637,8 +637,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="783">
+  <cellStyleXfs count="807">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1463,7 +1487,7 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="783">
+  <cellStyles count="807">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1855,6 +1879,18 @@
     <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2246,6 +2282,18 @@
     <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3073,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3088,7 +3136,7 @@
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -3126,11 +3174,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F2" s="9">
-        <f>$E$6+$E$7+$E$9+$E$4+$E$3+$E$2/2</f>
-        <v>1.8279999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <f>$E$6+$E$7+$E$9+$E$4+$E$3+$E$2/2+F5</f>
+        <v>1.8479999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -3148,11 +3196,17 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="F3" s="9">
-        <f>$E$6+$E$7+$E$9+$E$4 + $E$3/2</f>
-        <v>1.657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30">
+        <f>$E$6+$E$7+$E$9+$E$4 + $E$3/2+F5</f>
+        <v>1.677</v>
+      </c>
+      <c r="H3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -3170,11 +3224,11 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="F4" s="9">
-        <f>$E$6+$E$7+$E$9+$E$4/2</f>
-        <v>1.3699999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30">
+        <f>$E$6+$E$7+$E$9+$E$4/2+F5</f>
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -3192,10 +3246,11 @@
         <v>8.199999999999999E-2</v>
       </c>
       <c r="F5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <f>I3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -3213,11 +3268,11 @@
         <v>0.40899999999999997</v>
       </c>
       <c r="F6" s="9">
-        <f>E6/2</f>
-        <v>0.20449999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <f>E6/2+F5</f>
+        <v>0.22449999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -3235,11 +3290,11 @@
         <v>0.434</v>
       </c>
       <c r="F7">
-        <f>E6+E7/2</f>
-        <v>0.626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <f>E6+E7/2+F5</f>
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -3258,11 +3313,11 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F8" s="9">
-        <f>E9+E7+E6+E8/2</f>
-        <v>1.3815</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90">
+        <f>E9+E7+E6+E8/2+F5</f>
+        <v>1.4015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90">
       <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
@@ -3281,11 +3336,11 @@
         <v>0.37599999999999995</v>
       </c>
       <c r="F9" s="9">
-        <f>E6+E7+E9/2</f>
-        <v>1.0309999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <f>E6+E7+E9/2+F5</f>
+        <v>1.0509999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="10"/>
@@ -3293,7 +3348,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="10"/>
@@ -4149,7 +4204,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4206,7 +4261,7 @@
         <v>-8.5500000000000007E-2</v>
       </c>
       <c r="D2">
-        <f>K4</f>
+        <f>Height!I3</f>
         <v>0.02</v>
       </c>
       <c r="E2">
@@ -4271,7 +4326,7 @@
         <v>8.5500000000000007E-2</v>
       </c>
       <c r="D4">
-        <f>K4</f>
+        <f>Height!I3</f>
         <v>0.02</v>
       </c>
       <c r="E4">
@@ -4286,12 +4341,6 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="J4" t="s">
-        <v>165</v>
-      </c>
-      <c r="K4">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
@@ -4333,7 +4382,7 @@
       </c>
       <c r="D6">
         <f>Height!$F$6</f>
-        <v>0.20449999999999999</v>
+        <v>0.22449999999999998</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -4345,7 +4394,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>0.20449999999999999</v>
+        <v>0.22449999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -4388,7 +4437,7 @@
       </c>
       <c r="D8">
         <f>Height!$F$6</f>
-        <v>0.20449999999999999</v>
+        <v>0.22449999999999998</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -4400,7 +4449,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>0.20449999999999999</v>
+        <v>0.22449999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -4443,7 +4492,7 @@
       </c>
       <c r="D10">
         <f>Height!$F$7</f>
-        <v>0.626</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -4455,7 +4504,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>0.626</v>
+        <v>0.64600000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -4498,7 +4547,7 @@
       </c>
       <c r="D12">
         <f>Height!$F$7</f>
-        <v>0.626</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
@@ -4510,7 +4559,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>0.626</v>
+        <v>0.64600000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -4551,8 +4600,8 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <f>Height!$E$6+Height!$E$7</f>
-        <v>0.84299999999999997</v>
+        <f>Height!$E$6+Height!$E$7+D2</f>
+        <v>0.86299999999999999</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
@@ -4564,7 +4613,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0.84299999999999997</v>
+        <v>0.86299999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -4605,7 +4654,7 @@
       </c>
       <c r="D16">
         <f>Height!$F$9</f>
-        <v>1.0309999999999999</v>
+        <v>1.0509999999999999</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -4617,7 +4666,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>1.0309999999999999</v>
+        <v>1.0509999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4657,8 +4706,8 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f>Height!$E$6+Height!$E$7+Height!$E$9</f>
-        <v>1.2189999999999999</v>
+        <f>Height!$E$6+Height!$E$7+Height!$E$9+D2</f>
+        <v>1.2389999999999999</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -4670,7 +4719,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>1.2189999999999999</v>
+        <v>1.2389999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4711,7 +4760,8 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1.3815</v>
+        <f>Height!F8</f>
+        <v>1.4015</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -4723,7 +4773,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>1.3815</v>
+        <v>1.4015</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4739,7 +4789,7 @@
       </c>
       <c r="D21">
         <f>Height!$F$4</f>
-        <v>1.3699999999999999</v>
+        <v>1.39</v>
       </c>
       <c r="E21">
         <f t="shared" ref="E21:E30" si="3">B21+$K$2</f>
@@ -4751,7 +4801,7 @@
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G30" si="5">D21+$M$2</f>
-        <v>1.3699999999999999</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -4794,7 +4844,7 @@
       </c>
       <c r="D23">
         <f>Height!$F$4</f>
-        <v>1.3699999999999999</v>
+        <v>1.39</v>
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
@@ -4806,7 +4856,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="5"/>
-        <v>1.3699999999999999</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4849,7 +4899,7 @@
       </c>
       <c r="D25">
         <f>Height!$F$3</f>
-        <v>1.657</v>
+        <v>1.677</v>
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
@@ -4861,7 +4911,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="5"/>
-        <v>1.657</v>
+        <v>1.677</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4904,7 +4954,7 @@
       </c>
       <c r="D27">
         <f>Height!$F$3</f>
-        <v>1.657</v>
+        <v>1.677</v>
       </c>
       <c r="E27">
         <f t="shared" si="3"/>
@@ -4916,7 +4966,7 @@
       </c>
       <c r="G27">
         <f t="shared" si="5"/>
-        <v>1.657</v>
+        <v>1.677</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -4959,7 +5009,7 @@
       </c>
       <c r="D29">
         <f>Height!$F$2</f>
-        <v>1.8279999999999998</v>
+        <v>1.8479999999999999</v>
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
@@ -4971,7 +5021,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>1.8279999999999998</v>
+        <v>1.8479999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5014,7 +5064,7 @@
       </c>
       <c r="D31">
         <f>Height!$F$2</f>
-        <v>1.8279999999999998</v>
+        <v>1.8479999999999999</v>
       </c>
       <c r="E31">
         <f t="shared" ref="E31:E32" si="6">B31+$K$2</f>
@@ -5026,7 +5076,7 @@
       </c>
       <c r="G31">
         <f t="shared" ref="G31" si="8">D31+$M$2</f>
-        <v>1.8279999999999998</v>
+        <v>1.8479999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:7">

</xml_diff>

<commit_message>
Add two degrees of freedom at neck
</commit_message>
<xml_diff>
--- a/data/human_measurements.xlsx
+++ b/data/human_measurements.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="171">
   <si>
     <t>Pounds to Kilograms</t>
   </si>
@@ -495,9 +495,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Currently locking neck movement</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -523,6 +520,24 @@
   </si>
   <si>
     <t>Cylinder Radius</t>
+  </si>
+  <si>
+    <t>Noninvasive Measurement of Cervical Tri-Planar Motion in Normal Subjects. (misc)</t>
+  </si>
+  <si>
+    <t>Used Male Mean</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Flexion</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
   </si>
 </sst>
 </file>
@@ -637,8 +652,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="817">
+  <cellStyleXfs count="839">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1497,7 +1534,7 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="817">
+  <cellStyles count="839">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1906,6 +1943,17 @@
     <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="838" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2314,6 +2362,17 @@
     <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="837" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3220,7 +3279,7 @@
         <v>1.677</v>
       </c>
       <c r="H3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I3">
         <v>0.02</v>
@@ -5142,7 +5201,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5158,7 +5217,7 @@
         <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F1" t="s">
         <v>125</v>
@@ -5167,7 +5226,7 @@
         <v>126</v>
       </c>
       <c r="H1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I1" t="s">
         <v>42</v>
@@ -5179,7 +5238,7 @@
         <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -5193,26 +5252,26 @@
         <v>-39</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2">
         <f>RADIANS(C2)</f>
         <v>-0.68067840827778847</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" t="s">
         <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5223,20 +5282,20 @@
         <v>41.6</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F31" si="0">RADIANS(C3)</f>
         <v>0.7260569688296411</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
         <v>127</v>
@@ -5253,20 +5312,20 @@
         <v>-39</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>-0.68067840827778847</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
         <v>48</v>
@@ -5280,20 +5339,20 @@
         <v>41.6</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0.7260569688296411</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I5" t="s">
         <v>128</v>
@@ -5310,26 +5369,26 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
         <v>129</v>
       </c>
       <c r="J6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5340,20 +5399,20 @@
         <v>123.8</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>2.1607176139689801</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I7" t="s">
         <v>130</v>
@@ -5370,20 +5429,20 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I8" t="s">
         <v>131</v>
@@ -5397,20 +5456,20 @@
         <v>123.8</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>2.1607176139689801</v>
       </c>
       <c r="G9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I9" t="s">
         <v>132</v>
@@ -5448,7 +5507,7 @@
         <v>133</v>
       </c>
       <c r="J10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -5512,7 +5571,7 @@
         <v>135</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -5569,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I14" t="s">
         <v>137</v>
@@ -5597,7 +5656,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I15" t="s">
         <v>138</v>
@@ -5628,13 +5687,13 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:12">
       <c r="B17" t="s">
         <v>121</v>
       </c>
@@ -5656,13 +5715,13 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -5670,61 +5729,76 @@
         <v>120</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>-50.2</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>-44</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.87615528450115343</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I18" t="s">
         <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>167</v>
+      </c>
+      <c r="K18" t="s">
+        <v>169</v>
+      </c>
+      <c r="L18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="B19" t="s">
         <v>121</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>62.9</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F19">
         <f>RADIANS(C19)</f>
-        <v>0</v>
+        <v>1.0978120995044334</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="J19" t="s">
+        <v>168</v>
+      </c>
+      <c r="K19" t="s">
+        <v>170</v>
+      </c>
+      <c r="L19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -5756,7 +5830,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:12">
       <c r="B21" t="s">
         <v>121</v>
       </c>
@@ -5785,7 +5859,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -5817,7 +5891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:12">
       <c r="B23" t="s">
         <v>121</v>
       </c>
@@ -5846,7 +5920,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -5857,26 +5931,26 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:12">
       <c r="B25" t="s">
         <v>121</v>
       </c>
@@ -5884,26 +5958,26 @@
         <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
         <v>2.4609142453120048</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I25" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -5914,26 +5988,26 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I26" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
         <v>121</v>
       </c>
@@ -5941,26 +6015,26 @@
         <v>141</v>
       </c>
       <c r="D27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>2.4609142453120048</v>
       </c>
       <c r="G27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -5974,7 +6048,7 @@
         <v>-25.1</v>
       </c>
       <c r="E28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
@@ -5985,13 +6059,13 @@
         <v>-0.43807764225057672</v>
       </c>
       <c r="H28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I28" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
         <v>121</v>
       </c>
@@ -6002,7 +6076,7 @@
         <v>46.3</v>
       </c>
       <c r="E29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -6013,13 +6087,13 @@
         <v>0.80808744367337448</v>
       </c>
       <c r="H29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -6033,7 +6107,7 @@
         <v>-25.1</v>
       </c>
       <c r="E30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
@@ -6044,13 +6118,13 @@
         <v>-0.43807764225057672</v>
       </c>
       <c r="H30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
         <v>121</v>
       </c>
@@ -6061,7 +6135,7 @@
         <v>46.3</v>
       </c>
       <c r="E31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
@@ -6072,7 +6146,7 @@
         <v>0.80808744367337448</v>
       </c>
       <c r="H31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I31" t="s">
         <v>154</v>

</xml_diff>